<commit_message>
updated daily scrum report
</commit_message>
<xml_diff>
--- a/docs/deliverable3/Getana_Deliverable_3_DailyScrumReport.xlsx
+++ b/docs/deliverable3/Getana_Deliverable_3_DailyScrumReport.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sakshyam\Desktop\rn\RaiderNAV\docs\deliverable3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sakshyam\Desktop\software\RaiderNAV\docs\deliverable3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22E446A-8424-428F-8240-3A7A5849BDAB}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB911D4-9C6A-45FA-A138-D7B2698C9C6B}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="133">
   <si>
     <t>Daily Scrum Report — Sprint 1</t>
   </si>
@@ -375,9 +375,6 @@
     <t>Daily Scrum Report — Sprint 4</t>
   </si>
   <si>
-    <t>?? Mar 18</t>
-  </si>
-  <si>
     <t>Attended meeting, planned implementation of more user stories</t>
   </si>
   <si>
@@ -397,6 +394,39 @@
   </si>
   <si>
     <t>Impement code to show the shortest route possible at all times</t>
+  </si>
+  <si>
+    <t>Created a verificatin screen for delete schedule button, more tasks discussed and divided.</t>
+  </si>
+  <si>
+    <t>Implemented a quickfind feature in the homescreen of the application, more tasks discussed and divided.</t>
+  </si>
+  <si>
+    <t>Implemented a one time welcome screen with privacy notice, updated zenhub board, updated scrum report and sprint backlog.</t>
+  </si>
+  <si>
+    <t>Working on implementing code to show the shortest walking route during navigation.</t>
+  </si>
+  <si>
+    <t>Working on implementing a functionality to add temporary food locations, more tasks discussed and divided.</t>
+  </si>
+  <si>
+    <t>Implemented the app to determine location of buildings matching TTU database, more tasks discussed and divided.</t>
+  </si>
+  <si>
+    <t>Start with creation of  a Test plan document.Update SRS and Use Case models document.Update GRL and UCM Models document.</t>
+  </si>
+  <si>
+    <t>Start creating a Software Architecture and Design Pattern Document. Update SRS and Use Case models document.Update GRL and UCM Models document.</t>
+  </si>
+  <si>
+    <t>Update the domain model and detailed design document. Update SRS and Use Case models document.Update GRL and UCM Models document.</t>
+  </si>
+  <si>
+    <t>Update Configuration Management document, Update platform Document. Update SRS and Use Case models document.Update GRL and UCM Models document.</t>
+  </si>
+  <si>
+    <t>Start creating a Test plan document. Update SRS and Use Case models document.Update GRL and UCM Models document.</t>
   </si>
 </sst>
 </file>
@@ -1562,7 +1592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L83"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="B34" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
@@ -1997,7 +2027,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -2303,7 +2333,7 @@
   <dimension ref="A1:L56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2347,7 +2377,7 @@
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2355,7 +2385,7 @@
         <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2371,7 +2401,7 @@
         <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2379,7 +2409,7 @@
         <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2395,7 +2425,7 @@
         <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -2403,7 +2433,7 @@
         <v>33</v>
       </c>
       <c r="E17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -2419,7 +2449,7 @@
         <v>8</v>
       </c>
       <c r="E20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -2427,7 +2457,7 @@
         <v>33</v>
       </c>
       <c r="E21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -2443,7 +2473,7 @@
         <v>8</v>
       </c>
       <c r="E24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2451,7 +2481,7 @@
         <v>33</v>
       </c>
       <c r="E25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -2467,7 +2497,7 @@
         <v>8</v>
       </c>
       <c r="E28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -2475,7 +2505,7 @@
         <v>33</v>
       </c>
       <c r="E29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -2501,78 +2531,102 @@
       <c r="A32" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="4">
+        <v>43189</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>7</v>
       </c>
       <c r="C33" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>13</v>
       </c>
       <c r="C37" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>16</v>
       </c>
       <c r="C41" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>18</v>
       </c>
       <c r="C45" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>30</v>
       </c>
@@ -2584,11 +2638,17 @@
       <c r="C49" t="s">
         <v>8</v>
       </c>
+      <c r="E49" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
         <v>33</v>
       </c>
+      <c r="E50" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
@@ -2602,10 +2662,16 @@
       <c r="C53" t="s">
         <v>8</v>
       </c>
+      <c r="E53" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
         <v>33</v>
+      </c>
+      <c r="E54" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>